<commit_message>
V3 edits to tables
</commit_message>
<xml_diff>
--- a/AAJC Vis/case_studies/alone_and_AIC_tables.xlsx
+++ b/AAJC Vis/case_studies/alone_and_AIC_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anamkhan/Documents/Demo Advisors/AAJC/AAJC Vis/case_studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB797CA9-C79B-5D4F-B8F0-3C234023B3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926AD514-F97E-6148-B72C-8ADA6B6183B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17220" activeTab="6" xr2:uid="{1B42BBEE-F4C6-EA4B-BE1D-17B8B9AE08ED}"/>
+    <workbookView xWindow="-20" yWindow="740" windowWidth="29400" windowHeight="17220" activeTab="6" xr2:uid="{1B42BBEE-F4C6-EA4B-BE1D-17B8B9AE08ED}"/>
   </bookViews>
   <sheets>
     <sheet name="LA  - CA" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Arkansas" sheetId="6" r:id="rId6"/>
     <sheet name="Utah" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="19">
   <si>
     <t>count</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>Arkansas NHPI Population by Race Group</t>
+  </si>
+  <si>
+    <t>Salt Lake County NHPI Population by Race Group</t>
+  </si>
+  <si>
+    <t>Utah County NHPI Population by Race Group</t>
   </si>
 </sst>
 </file>
@@ -346,39 +352,6 @@
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -436,6 +409,39 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -761,7 +767,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -776,159 +782,159 @@
   <sheetData>
     <row r="1" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="9"/>
-      <c r="C4" s="10">
+      <c r="B4" s="26"/>
+      <c r="C4" s="31">
         <v>2000</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10">
+      <c r="D4" s="32"/>
+      <c r="E4" s="31">
         <v>2010</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10">
+      <c r="F4" s="32"/>
+      <c r="G4" s="31">
         <v>2020</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="12"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="16"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="4">
         <v>1173799</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="12">
         <f>C7/$C$9</f>
         <v>0.1233067887703956</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="4">
         <v>1393578</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="12">
         <f>E7/$E$9</f>
         <v>0.1419323824514786</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="4">
         <v>1489041</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="12">
         <f>G7/$G$9</f>
         <v>0.14869579206489628</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="7">
         <v>1258275</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="13">
         <f>C8/$C$9</f>
         <v>0.13218093527091904</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="7">
         <v>1535944</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="13">
         <f>E8/$E$9</f>
         <v>0.15643199823192805</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="7">
         <v>1639661</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="13">
         <f>G8/$G$9</f>
         <v>0.16373672122723276</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="17">
         <v>9519338</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="17">
         <v>9818605</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="17">
         <v>10014009</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="14" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
@@ -938,151 +944,151 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="J11" s="21"/>
+      <c r="J11" s="10"/>
     </row>
     <row r="12" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="2:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="B13" s="5" t="s">
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
+    </row>
+    <row r="13" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="2:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="B14" s="9"/>
-      <c r="C14" s="10">
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="30"/>
+    </row>
+    <row r="14" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="26"/>
+      <c r="C14" s="31">
         <v>2000</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="10">
+      <c r="D14" s="32"/>
+      <c r="E14" s="31">
         <v>2010</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="10">
+      <c r="F14" s="32"/>
+      <c r="G14" s="31">
         <v>2020</v>
       </c>
-      <c r="H14" s="11"/>
+      <c r="H14" s="32"/>
     </row>
     <row r="15" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="12"/>
-      <c r="C15" s="13" t="s">
+      <c r="B15" s="27"/>
+      <c r="C15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="16"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" spans="2:8" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="4">
         <v>33598</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="12">
         <f>C17/$C$19</f>
         <v>3.5294471107129508E-3</v>
       </c>
-      <c r="E17" s="15">
-        <v>35837</v>
-      </c>
-      <c r="F17" s="23">
+      <c r="E17" s="4">
+        <v>36443</v>
+      </c>
+      <c r="F17" s="12">
         <f>E17/$E$19</f>
-        <v>3.6499074970426045E-3</v>
-      </c>
-      <c r="G17" s="15">
+        <v>3.711627059037409E-3</v>
+      </c>
+      <c r="G17" s="4">
         <v>21327</v>
       </c>
-      <c r="H17" s="23">
+      <c r="H17" s="12">
         <f>G17/$G$19</f>
         <v>2.1297164801829119E-3</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="7">
         <v>53480</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="13">
         <f>C18/$C$19</f>
         <v>5.6180377248922142E-3</v>
       </c>
-      <c r="E18" s="18">
-        <v>60508</v>
-      </c>
-      <c r="F18" s="24">
+      <c r="E18" s="7">
+        <v>62945</v>
+      </c>
+      <c r="F18" s="13">
         <f>E18/$E$19</f>
-        <v>6.1625862329730136E-3</v>
-      </c>
-      <c r="G18" s="18">
+        <v>6.4107884979587226E-3</v>
+      </c>
+      <c r="G18" s="7">
         <v>44206</v>
       </c>
-      <c r="H18" s="24">
+      <c r="H18" s="13">
         <f>G18/$G$19</f>
         <v>4.4144158448429591E-3</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="28">
+      <c r="C19" s="17">
         <v>9519338</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E19" s="17">
         <v>9818605</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G19" s="28">
+      <c r="G19" s="17">
         <v>10014009</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="14" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1097,18 +1103,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
     <mergeCell ref="B12:H12"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="C13:H13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1132,159 +1138,159 @@
   <sheetData>
     <row r="1" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="9"/>
-      <c r="C4" s="10">
+      <c r="B4" s="26"/>
+      <c r="C4" s="31">
         <v>2000</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10">
+      <c r="D4" s="32"/>
+      <c r="E4" s="31">
         <v>2010</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10">
+      <c r="F4" s="32"/>
+      <c r="G4" s="31">
         <v>2020</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="12"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="4">
         <v>191741</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="12">
         <f>C7/$C$9</f>
         <v>0.11038413755862003</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="4">
         <v>286648</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="12">
         <f>E7/$E$9</f>
         <v>0.14842622572231753</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="4">
         <v>453230</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="12">
         <f>G7/$G$9</f>
         <v>0.19968938284115567</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="7">
         <v>218242</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="13">
         <f>C8/$C$9</f>
         <v>0.12564060346544742</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="7">
         <v>333338</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="13">
         <f>E8/$E$9</f>
         <v>0.17260229002060326</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="7">
         <v>527853</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="13">
         <f>G8/$G$9</f>
         <v>0.23256765836518445</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="17">
         <v>1737034</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="17">
         <v>1931249</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="17">
         <v>2269675</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="14" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1343,159 +1349,159 @@
   <sheetData>
     <row r="1" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="9"/>
-      <c r="C4" s="10">
+      <c r="B4" s="26"/>
+      <c r="C4" s="31">
         <v>2000</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10">
+      <c r="D4" s="32"/>
+      <c r="E4" s="31">
         <v>2010</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10">
+      <c r="F4" s="32"/>
+      <c r="G4" s="31">
         <v>2020</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="12"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="4">
         <v>181356</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="12">
         <f>C7/$C$9</f>
         <v>5.3330933741263985E-2</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="4">
         <v>261637</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="12">
         <f>E7/$E$9</f>
         <v>6.393148960075104E-2</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="4">
         <v>348281</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="12">
         <f>G7/$G$9</f>
         <v>7.3614526716048651E-2</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="7">
         <v>194941</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="13">
         <f>C8/$C$9</f>
         <v>5.7325842842010977E-2</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="7">
         <v>285796</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="13">
         <f>E8/$E$9</f>
         <v>6.9834786371714419E-2</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="7">
         <v>382276</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="13">
         <f>G8/$G$9</f>
         <v>8.0799890935492363E-2</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="17">
         <v>3400578</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="17">
         <v>4092459</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="17">
         <v>4731145</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="14" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1554,159 +1560,159 @@
   <sheetData>
     <row r="1" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="9"/>
-      <c r="C4" s="10">
+      <c r="B4" s="26"/>
+      <c r="C4" s="31">
         <v>2000</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10">
+      <c r="D4" s="32"/>
+      <c r="E4" s="31">
         <v>2010</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10">
+      <c r="F4" s="32"/>
+      <c r="G4" s="31">
         <v>2020</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="12"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="4">
         <v>838074</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="12">
         <f>C7/$C$9</f>
         <v>0.10465096241663938</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="4">
         <v>1086296</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="12">
         <f>E7/$E$9</f>
         <v>0.13287808283975319</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="4">
         <v>1420318</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="12">
         <f>G7/$G$9</f>
         <v>0.1613229609992515</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="7">
         <v>891718</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="13">
         <f>C8/$C$9</f>
         <v>0.1113495310727225</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="7">
         <v>1167545</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="13">
         <f>E8/$E$9</f>
         <v>0.14281663674462544</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="7">
         <v>1531522</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="13">
         <f>G8/$G$9</f>
         <v>0.17395376519588968</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="17">
         <v>8008278</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="17">
         <v>8175133</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="17">
         <v>8804190</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="14" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1768,159 +1774,159 @@
   <sheetData>
     <row r="1" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="9"/>
-      <c r="C4" s="10">
+      <c r="B4" s="26"/>
+      <c r="C4" s="31">
         <v>2000</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10">
+      <c r="D4" s="32"/>
+      <c r="E4" s="31">
         <v>2010</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10">
+      <c r="F4" s="32"/>
+      <c r="G4" s="31">
         <v>2020</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="12"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="4">
         <v>115964</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="12">
         <f>C7/$C$9</f>
         <v>9.5716432927760359E-2</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="4">
         <v>138292</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="12">
         <f>E7/$E$9</f>
         <v>0.1016627937493246</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="4">
         <v>149949</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="12">
         <f>G7/$G$9</f>
         <v>0.10303854058797296</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="7">
         <v>283430</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="13">
         <f>C8/$C$9</f>
         <v>0.23394250443857678</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="7">
         <v>358951</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="13">
         <f>E8/$E$9</f>
         <v>0.26387615682117416</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="7">
         <v>345220</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="13">
         <f>G8/$G$9</f>
         <v>0.23722042148850628</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="17">
         <v>1211537</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="17">
         <v>1360301</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="17">
         <v>1455271</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="14" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1955,7 +1961,7 @@
   <dimension ref="A1:J163"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1968,159 +1974,159 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="9"/>
-      <c r="C4" s="10">
+      <c r="B4" s="26"/>
+      <c r="C4" s="31">
         <v>2000</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10">
+      <c r="D4" s="32"/>
+      <c r="E4" s="31">
         <v>2010</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10">
+      <c r="F4" s="32"/>
+      <c r="G4" s="31">
         <v>2020</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="12"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="4">
         <v>1930</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="20">
         <f>C7/$C$9</f>
         <v>7.2192713398668365E-4</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="4">
         <v>6685</v>
       </c>
-      <c r="F7" s="31">
+      <c r="F7" s="20">
         <f>E7/$E$9</f>
         <v>2.2925884747101942E-3</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="4">
         <v>14461</v>
       </c>
-      <c r="H7" s="31">
+      <c r="H7" s="20">
         <f>G7/$G$9</f>
         <v>4.8018876821170941E-3</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="7">
         <v>3223</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="21">
         <f>C8/$C$9</f>
         <v>1.2055809082067779E-3</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="7">
         <v>8594</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="21">
         <f>E8/$E$9</f>
         <v>2.9472708080268374E-3</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="7">
         <v>17252</v>
       </c>
-      <c r="H8" s="32">
+      <c r="H8" s="21">
         <f>G8/$G$9</f>
         <v>5.728660970325988E-3</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="17">
         <v>2673400</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="17">
         <v>2915918</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="17">
         <v>3011524</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="14" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2602,10 +2608,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47DF1251-5C24-1B4C-BF61-5C7BF7578CF5}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2618,188 +2624,318 @@
   <sheetData>
     <row r="1" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4"/>
+      <c r="B2" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="2:10" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="9"/>
-      <c r="C4" s="10">
+      <c r="B4" s="26"/>
+      <c r="C4" s="31">
         <v>2000</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10">
+      <c r="D4" s="32"/>
+      <c r="E4" s="31">
         <v>2010</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10">
+      <c r="F4" s="32"/>
+      <c r="G4" s="31">
         <v>2020</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="12"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
+      <c r="B6" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="15">
-        <v>838074</v>
-      </c>
-      <c r="D7" s="23">
+      <c r="C7" s="4">
+        <v>11699</v>
+      </c>
+      <c r="D7" s="12">
         <f>C7/$C$9</f>
-        <v>0.10465096241663938</v>
-      </c>
-      <c r="E7" s="15">
-        <v>1086296</v>
-      </c>
-      <c r="F7" s="23">
+        <v>1.3022227614602616E-2</v>
+      </c>
+      <c r="E7" s="4">
+        <v>16564</v>
+      </c>
+      <c r="F7" s="12">
         <f>E7/$E$9</f>
-        <v>0.13287808283975319</v>
-      </c>
-      <c r="G7" s="15">
-        <v>1420318</v>
-      </c>
-      <c r="H7" s="23">
+        <v>1.608694174262253E-2</v>
+      </c>
+      <c r="G7" s="4">
+        <v>21314</v>
+      </c>
+      <c r="H7" s="12">
         <f>G7/$G$9</f>
-        <v>0.1613229609992515</v>
+        <v>1.7982886137636492E-2</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="18">
-        <v>891718</v>
-      </c>
-      <c r="D8" s="24">
+      <c r="C8" s="7">
+        <v>14404</v>
+      </c>
+      <c r="D8" s="13">
         <f>C8/$C$9</f>
-        <v>0.1113495310727225</v>
-      </c>
-      <c r="E8" s="18">
-        <v>1167545</v>
-      </c>
-      <c r="F8" s="24">
+        <v>1.6033179464974449E-2</v>
+      </c>
+      <c r="E8" s="7">
+        <v>21451</v>
+      </c>
+      <c r="F8" s="13">
         <f>E8/$E$9</f>
-        <v>0.14281663674462544</v>
-      </c>
-      <c r="G8" s="18">
-        <v>1531522</v>
-      </c>
-      <c r="H8" s="24">
+        <v>2.0833191700132567E-2</v>
+      </c>
+      <c r="G8" s="7">
+        <v>28610</v>
+      </c>
+      <c r="H8" s="13">
         <f>G8/$G$9</f>
-        <v>0.17395376519588968</v>
+        <v>2.4138611823110633E-2</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="28">
-        <v>8008278</v>
-      </c>
-      <c r="D9" s="25" t="s">
+      <c r="C9" s="17">
+        <v>898387</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="28">
-        <v>8175133</v>
-      </c>
-      <c r="F9" s="25" t="s">
+      <c r="E9" s="17">
+        <v>1029655</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="28">
-        <v>8804190</v>
-      </c>
-      <c r="H9" s="25" t="s">
+      <c r="G9" s="17">
+        <v>1185238</v>
+      </c>
+      <c r="H9" s="14" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-    </row>
-    <row r="11" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="2:10" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
+    </row>
     <row r="13" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13"/>
+      <c r="B13" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="30"/>
       <c r="J13"/>
     </row>
     <row r="14" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="31">
+        <v>2000</v>
+      </c>
+      <c r="D14" s="32"/>
+      <c r="E14" s="31">
+        <v>2010</v>
+      </c>
+      <c r="F14" s="32"/>
+      <c r="G14" s="31">
+        <v>2020</v>
+      </c>
+      <c r="H14" s="32"/>
       <c r="J14"/>
     </row>
-    <row r="15" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="27"/>
+      <c r="C15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="2:8" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2203</v>
+      </c>
+      <c r="D17" s="12">
+        <f>C17/$C$19</f>
+        <v>5.9777063841795642E-3</v>
+      </c>
+      <c r="E17" s="4">
+        <v>4089</v>
+      </c>
+      <c r="F17" s="12">
+        <f>E17/$E$19</f>
+        <v>7.9157664877924135E-3</v>
+      </c>
+      <c r="G17" s="4">
+        <v>6652</v>
+      </c>
+      <c r="H17" s="12">
+        <f>G17/$G$19</f>
+        <v>1.0087974049096223E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="7">
+        <v>3630</v>
+      </c>
+      <c r="D18" s="13">
+        <f>C18/$C$19</f>
+        <v>9.8497840102459468E-3</v>
+      </c>
+      <c r="E18" s="7">
+        <v>7596</v>
+      </c>
+      <c r="F18" s="13">
+        <f>E18/$E$19</f>
+        <v>1.4704857481357586E-2</v>
+      </c>
+      <c r="G18" s="7">
+        <v>13138</v>
+      </c>
+      <c r="H18" s="13">
+        <f>G18/$G$19</f>
+        <v>1.9924203706708686E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="17">
+        <v>368536</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="17">
+        <v>516564</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="17">
+        <v>659399</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="12">
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:H3"/>

</xml_diff>